<commit_message>
adds data on porometer moves files, adds scripts to analyze porometer data and traits
</commit_message>
<xml_diff>
--- a/data/raw/Flower_traits.xlsx
+++ b/data/raw/Flower_traits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gretchen/GitHub/CApoppy/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48F8A7E-EC93-5449-8FE4-BBF33531B8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0BFA52-1276-2448-9F52-38CF920BCA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="33520" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10740" yWindow="2820" windowWidth="33520" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Petal_2025_low" sheetId="1" r:id="rId1"/>
@@ -221,9 +221,6 @@
     <t>wet_wgt</t>
   </si>
   <si>
-    <t>Top_gws</t>
-  </si>
-  <si>
     <t>Bottom_gsw</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>Bottom_time</t>
+  </si>
+  <si>
+    <t>Top_gsw</t>
   </si>
 </sst>
 </file>
@@ -607,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,7 +620,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -638,13 +638,13 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" t="s">
         <v>63</v>
       </c>
-      <c r="I1" t="s">
-        <v>64</v>
-      </c>
       <c r="J1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K1" t="s">
         <v>61</v>
@@ -1262,16 +1262,6 @@
       </c>
       <c r="L17">
         <v>3.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H20">
-        <f>AVERAGE(H3:H17)</f>
-        <v>4.4923415843549069E-3</v>
-      </c>
-      <c r="J20">
-        <f>AVERAGE(J3:J17)</f>
-        <v>9.6330054365833459E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>